<commit_message>
baaam - nice coef table for mmdcev
</commit_message>
<xml_diff>
--- a/data-raw/mpp_coef_labels.xlsx
+++ b/data-raw/mpp_coef_labels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\daniehei\github\myThesis\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0A3880-850C-4299-B954-617FB4558225}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0CF0BF-4DD9-49D4-B594-ED3EF7922B8C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="9885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -88,9 +88,6 @@
     <t>Sigma</t>
   </si>
   <si>
-    <t>Gammama</t>
-  </si>
-  <si>
     <t>ASC</t>
   </si>
   <si>
@@ -137,6 +134,9 @@
   </si>
   <si>
     <t>Home and office</t>
+  </si>
+  <si>
+    <t>Gamma</t>
   </si>
 </sst>
 </file>
@@ -491,7 +491,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,7 +531,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -542,7 +542,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -553,7 +553,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -564,7 +564,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -575,7 +575,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -586,7 +586,7 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -597,7 +597,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -608,7 +608,7 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -619,7 +619,7 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -630,7 +630,7 @@
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -641,7 +641,7 @@
         <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -652,7 +652,7 @@
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -663,7 +663,7 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -674,7 +674,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -685,7 +685,7 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -696,7 +696,7 @@
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -707,7 +707,7 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>